<commit_message>
Added spreadsheets given to us from the client
</commit_message>
<xml_diff>
--- a/Veterans Cemetary Project.xlsx
+++ b/Veterans Cemetary Project.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OK\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Repositories\VCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -369,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -378,63 +378,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="15">
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFDA1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -574,35 +527,12 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <color auto="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFBFDA1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -627,56 +557,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:G16" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:G16" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A2:G16"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="Data Type and length"/>
-    <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="18"/>
-    <tableColumn id="6" name="Default Value"/>
-    <tableColumn id="7" name="Notes"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A20:G37" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A20:G37"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="Data Type and length"/>
-    <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="16"/>
-    <tableColumn id="6" name="Default Value"/>
-    <tableColumn id="7" name="Notes"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A40:G42" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A40:G42"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="Data Type and length"/>
-    <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="14"/>
-    <tableColumn id="6" name="Default Value"/>
-    <tableColumn id="7" name="Notes"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A46:G48" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A46:G48"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
@@ -690,9 +572,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A52:G54" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A52:G54"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A20:G37" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A20:G37"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
@@ -706,9 +588,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A58:G60" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A58:G60"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A40:G42" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A40:G42"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
@@ -722,15 +604,63 @@
 </table>
 </file>
 
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A46:G48" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A46:G48"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="Data Type and length"/>
+    <tableColumn id="4" name="Domain Characteristics"/>
+    <tableColumn id="5" name="Required" dataDxfId="6"/>
+    <tableColumn id="6" name="Default Value"/>
+    <tableColumn id="7" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A52:G54" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A52:G54"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="Data Type and length"/>
+    <tableColumn id="4" name="Domain Characteristics"/>
+    <tableColumn id="5" name="Required" dataDxfId="4"/>
+    <tableColumn id="6" name="Default Value"/>
+    <tableColumn id="7" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A58:G60" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A58:G60"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Description"/>
+    <tableColumn id="3" name="Data Type and length"/>
+    <tableColumn id="4" name="Domain Characteristics"/>
+    <tableColumn id="5" name="Required" dataDxfId="2"/>
+    <tableColumn id="6" name="Default Value"/>
+    <tableColumn id="7" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A64:G67" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A64:G67" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A64:G67"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="6"/>
+    <tableColumn id="5" name="Required" dataDxfId="0"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
   </tableColumns>
@@ -1033,25 +963,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1066,7 +996,7 @@
       <c r="D2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1279,15 +1209,15 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1302,7 +1232,7 @@
       <c r="D20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1551,15 +1481,15 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1574,7 +1504,7 @@
       <c r="D40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -1613,15 +1543,15 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1636,7 +1566,7 @@
       <c r="D46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F46" s="1" t="s">
@@ -1675,15 +1605,15 @@
       </c>
     </row>
     <row r="51" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
@@ -1698,7 +1628,7 @@
       <c r="D52" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -1737,15 +1667,15 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -1760,7 +1690,7 @@
       <c r="D58" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E58" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F58" s="1" t="s">
@@ -1799,15 +1729,15 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -1822,7 +1752,7 @@
       <c r="D64" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="E64" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F64" s="1" t="s">
@@ -1907,7 +1837,7 @@
     <mergeCell ref="A63:G63"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:H18 A20:H38 A19 H19 A40:H44 A39 H39 A46:H50 A45 H45 A52:H56 A51 H51 A58:H62 A57 H57 A64:H73 A63 H63">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added SQL file and Updated Data Dictionary
</commit_message>
<xml_diff>
--- a/Veterans Cemetary Project.xlsx
+++ b/Veterans Cemetary Project.xlsx
@@ -269,9 +269,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>GPSgrave</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -366,6 +363,9 @@
   </si>
   <si>
     <t>Dropdown using unique with option for adding new unit</t>
+  </si>
+  <si>
+    <t>gpsGrave</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -488,15 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -506,18 +497,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,62 +591,6 @@
           <bgColor rgb="FFFBFDA1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFDA1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFDA1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFDA1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFDA1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBFDA1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -770,6 +713,12 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -788,6 +737,56 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -810,31 +809,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:H17" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:H17" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A2:H17"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="26"/>
+    <tableColumn id="5" name="Required" dataDxfId="21"/>
     <tableColumn id="6" name="Default Value"/>
-    <tableColumn id="7" name="Notes" dataDxfId="13"/>
-    <tableColumn id="8" name="User Interface Notes" dataDxfId="12"/>
+    <tableColumn id="7" name="Notes" dataDxfId="20"/>
+    <tableColumn id="8" name="User Interface Notes" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A21:H37" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A21:H37" totalsRowShown="0" headerRowDxfId="18">
   <autoFilter ref="A21:H37"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="24"/>
+    <tableColumn id="5" name="Required" dataDxfId="17"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -844,14 +843,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A40:H42" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A40:H42" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A40:H42"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="22"/>
+    <tableColumn id="5" name="Required" dataDxfId="15"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -861,14 +860,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A46:H48" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A46:H48" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A46:H48"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="20"/>
+    <tableColumn id="5" name="Required" dataDxfId="13"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -878,14 +877,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A52:H54" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A52:H54" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A52:H54"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="18"/>
+    <tableColumn id="5" name="Required" dataDxfId="11"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -895,14 +894,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A58:H60" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A58:H60" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A58:H60"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="16"/>
+    <tableColumn id="5" name="Required" dataDxfId="9"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -912,14 +911,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A78:H81" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A78:H81" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A78:H81"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="14"/>
+    <tableColumn id="5" name="Required" dataDxfId="7"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -1217,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,16 +1233,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1268,7 +1267,7 @@
         <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1279,17 +1278,17 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1298,16 +1297,16 @@
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1316,30 +1315,30 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
-        <v>98</v>
+        <v>87</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
         <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
       </c>
       <c r="C6" t="s">
         <v>50</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H6" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1352,12 +1351,12 @@
         <v>51</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1370,12 +1369,12 @@
         <v>52</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H8" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1388,12 +1387,12 @@
         <v>50</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1406,12 +1405,12 @@
         <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H10" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1424,10 +1423,10 @@
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1440,12 +1439,12 @@
         <v>54</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1458,12 +1457,12 @@
         <v>50</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1473,19 +1472,19 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>94</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1496,19 +1495,19 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>94</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1519,15 +1518,15 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1537,27 +1536,27 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" s="14"/>
+        <v>88</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1582,7 +1581,7 @@
         <v>33</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1593,15 +1592,15 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1610,15 +1609,15 @@
         <v>49</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>99</v>
+        <v>87</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -1627,10 +1626,10 @@
         <v>49</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>98</v>
+        <v>87</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1644,10 +1643,10 @@
         <v>51</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1661,12 +1660,12 @@
         <v>49</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
@@ -1675,15 +1674,15 @@
         <v>55</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
@@ -1692,10 +1691,10 @@
         <v>49</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1709,7 +1708,7 @@
         <v>50</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1723,7 +1722,7 @@
         <v>50</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1737,10 +1736,10 @@
         <v>56</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1754,10 +1753,10 @@
         <v>55</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1771,13 +1770,13 @@
         <v>57</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F33" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1791,15 +1790,15 @@
         <v>57</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
@@ -1808,15 +1807,15 @@
         <v>50</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
         <v>33</v>
@@ -1825,40 +1824,40 @@
         <v>52</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
         <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1883,7 +1882,7 @@
         <v>33</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1894,10 +1893,10 @@
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1911,23 +1910,23 @@
         <v>50</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1952,7 +1951,7 @@
         <v>33</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1963,10 +1962,10 @@
         <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1980,23 +1979,23 @@
         <v>58</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
@@ -2021,7 +2020,7 @@
         <v>33</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2032,10 +2031,10 @@
         <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2049,23 +2048,23 @@
         <v>58</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -2090,7 +2089,7 @@
         <v>33</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2101,10 +2100,10 @@
         <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2118,10 +2117,10 @@
         <v>50</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
@@ -2137,43 +2136,43 @@
       <c r="H62" s="15"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F63" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H63" s="11" t="s">
-        <v>100</v>
+      <c r="H63" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2181,13 +2180,13 @@
         <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>110</v>
-      </c>
-      <c r="C65" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2197,75 +2196,75 @@
       <c r="A67" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G68" s="9" t="s">
+      <c r="G68" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H68" s="11" t="s">
-        <v>100</v>
+      <c r="H68" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B69" t="s">
         <v>106</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>110</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" t="s">
         <v>107</v>
       </c>
-      <c r="C69" t="s">
-        <v>49</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" t="s">
-        <v>108</v>
-      </c>
-      <c r="C70" s="12" t="s">
+      <c r="C70" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
-      <c r="C71" s="17"/>
+      <c r="A71" s="12"/>
+      <c r="C71" s="13"/>
       <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B72" s="18"/>
@@ -2277,72 +2276,73 @@
       <c r="H72" s="18"/>
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E73" s="10" t="s">
+      <c r="E73" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F73" s="9" t="s">
+      <c r="F73" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G73" s="9" t="s">
+      <c r="G73" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H73" s="11" t="s">
-        <v>100</v>
+      <c r="H73" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
         <v>112</v>
       </c>
-      <c r="C74" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H74" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="20" t="s">
-        <v>49</v>
+      <c r="C75" t="s">
+        <v>110</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
@@ -2367,7 +2367,7 @@
         <v>33</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
         <v>49</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>50</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2409,28 +2409,28 @@
         <v>58</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
+      <c r="A84" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2439,36 +2439,36 @@
     <mergeCell ref="A72:H72"/>
     <mergeCell ref="A84:F84"/>
     <mergeCell ref="A85:F85"/>
-    <mergeCell ref="A77:G77"/>
     <mergeCell ref="A62:H62"/>
     <mergeCell ref="A57:H57"/>
     <mergeCell ref="A51:H51"/>
     <mergeCell ref="A45:H45"/>
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A77:H77"/>
   </mergeCells>
-  <conditionalFormatting sqref="A20 A41:H44 A39 A45 A51 A57 A77 H77 A62 A3:H19 A47:H50 A53:H56 A59:H61 A79:H87 A21:G21 A40:G40 A46:G46 A52:G52 A58:G58 A78:G78 A67 A64:H66 A69:H71 A72 A74:B74 A22:H38 A76:H76 A75:G75 D74:H74">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="A20 A39 A45 A51 A57 A77 A62 A3:H19 A79:H87 A21:G21 A40:G40 A46:G46 A52:G52 A58:G58 A78:G78 A67 A72 A74:B74 A22:H38 A76:H76 D74:H74 A41:H44 A47:H50 A53:H56 A59:H61 A64:H66 A69:H71 A75:G75">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:G63">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:G68">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:G73">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Data Dictionary with UI Notes
</commit_message>
<xml_diff>
--- a/Veterans Cemetary Project.xlsx
+++ b/Veterans Cemetary Project.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="119">
   <si>
     <t>Country</t>
   </si>
@@ -302,9 +302,6 @@
     <t>County within the state</t>
   </si>
   <si>
-    <t>Dropdown</t>
-  </si>
-  <si>
     <t>Not Required</t>
   </si>
   <si>
@@ -314,27 +311,9 @@
     <t>If month/day is missing then will default to January 1st</t>
   </si>
   <si>
-    <t>Dropdown - Linked to Country</t>
-  </si>
-  <si>
-    <t>Dropdown - Linked to State</t>
-  </si>
-  <si>
     <t>User Interface Notes</t>
   </si>
   <si>
-    <t>Dropdown using unique with option for adding new rank</t>
-  </si>
-  <si>
-    <t>Dropdown using unique with option for adding new service</t>
-  </si>
-  <si>
-    <t>Dropdown using unique with option for adding new period</t>
-  </si>
-  <si>
-    <t>Dropdown using unique with option for adding new award</t>
-  </si>
-  <si>
     <t>sID</t>
   </si>
   <si>
@@ -362,10 +341,43 @@
     <t>Person ID Number</t>
   </si>
   <si>
-    <t>Dropdown using unique with option for adding new unit</t>
-  </si>
-  <si>
     <t>gpsGrave</t>
+  </si>
+  <si>
+    <t>Ignore in UI - this is used in database only</t>
+  </si>
+  <si>
+    <t>Dropdown - Linked to State - Content generated by our code</t>
+  </si>
+  <si>
+    <t>Dropdown - Linked to Country - Content generated by code</t>
+  </si>
+  <si>
+    <t>textbox (on upload page), label (when viewing veteran data)</t>
+  </si>
+  <si>
+    <t>Dropdown (when editing information), label (when viewing veteran data)</t>
+  </si>
+  <si>
+    <t>textbox (register page and login page)</t>
+  </si>
+  <si>
+    <t>label (when viewing veteran data), textbox when editing data</t>
+  </si>
+  <si>
+    <t>textbox (may need more than one depending on how we want to set it up for them to enter the data - for example do we want to do it in terms of latitude and longitude or do we want to do degrees/minutes/seconds)</t>
+  </si>
+  <si>
+    <t>textarea</t>
+  </si>
+  <si>
+    <t>image (when viewing veteran data), textbox and browse button (when uploading image)</t>
+  </si>
+  <si>
+    <t>Dropdown - Content generated by our code but we need a textbox so that if the user selects "Other" then we need the textbox so they can add their answer</t>
+  </si>
+  <si>
+    <t>textbox (may need more than one depending on whether or not we want to just check the format in the code or if we want to just use multiple textboxes and then combine it all into one format ourselves which might be easier)</t>
   </si>
 </sst>
 </file>
@@ -413,7 +425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +436,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -476,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -517,11 +535,282 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFBFDA1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -809,31 +1098,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:H17" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:H17" totalsRowShown="0" headerRowDxfId="49">
   <autoFilter ref="A2:H17"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="21"/>
+    <tableColumn id="5" name="Required" dataDxfId="48"/>
     <tableColumn id="6" name="Default Value"/>
-    <tableColumn id="7" name="Notes" dataDxfId="20"/>
-    <tableColumn id="8" name="User Interface Notes" dataDxfId="19"/>
+    <tableColumn id="7" name="Notes" dataDxfId="47"/>
+    <tableColumn id="8" name="User Interface Notes" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A21:H37" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A21:H37" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="A21:H37"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="17"/>
+    <tableColumn id="5" name="Required" dataDxfId="44"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -843,14 +1132,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A40:H42" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A40:H42" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A40:H42"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="15"/>
+    <tableColumn id="5" name="Required" dataDxfId="42"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -860,14 +1149,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A46:H48" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A46:H48" totalsRowShown="0" headerRowDxfId="41">
   <autoFilter ref="A46:H48"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="13"/>
+    <tableColumn id="5" name="Required" dataDxfId="40"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -877,14 +1166,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A52:H54" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A52:H54" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A52:H54"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="11"/>
+    <tableColumn id="5" name="Required" dataDxfId="38"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -894,14 +1183,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A58:H60" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A58:H60" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A58:H60"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="9"/>
+    <tableColumn id="5" name="Required" dataDxfId="36"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -911,14 +1200,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A78:H81" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A78:H81" totalsRowShown="0" headerRowDxfId="35">
   <autoFilter ref="A78:H81"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Data Type and length"/>
     <tableColumn id="4" name="Domain Characteristics"/>
-    <tableColumn id="5" name="Required" dataDxfId="7"/>
+    <tableColumn id="5" name="Required" dataDxfId="34"/>
     <tableColumn id="6" name="Default Value"/>
     <tableColumn id="7" name="Notes"/>
     <tableColumn id="8" name="User Interface Notes"/>
@@ -1216,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1518,7 @@
     <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.5703125" customWidth="1"/>
-    <col min="8" max="8" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="207.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1267,7 +1556,7 @@
         <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1278,17 +1567,19 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="H3" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1301,12 +1592,12 @@
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1319,7 +1610,7 @@
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1336,9 +1627,11 @@
         <v>88</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1354,9 +1647,11 @@
         <v>88</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1372,9 +1667,11 @@
         <v>88</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1390,9 +1687,11 @@
         <v>88</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1408,9 +1707,11 @@
         <v>88</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1426,7 +1727,9 @@
         <v>87</v>
       </c>
       <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1442,9 +1745,11 @@
         <v>88</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1460,9 +1765,11 @@
         <v>88</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1475,16 +1782,16 @@
         <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1498,16 +1805,16 @@
         <v>89</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1524,9 +1831,11 @@
         <v>88</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H16" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1542,9 +1851,11 @@
         <v>88</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
@@ -1581,7 +1892,7 @@
         <v>33</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,15 +1903,18 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="H22" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
         <v>0</v>
@@ -1612,12 +1926,12 @@
         <v>87</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
@@ -1629,7 +1943,7 @@
         <v>87</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1646,7 +1960,10 @@
         <v>88</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H25" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1662,6 +1979,9 @@
       <c r="E26" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="H26" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1677,7 +1997,10 @@
         <v>88</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1694,7 +2017,10 @@
         <v>88</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1710,6 +2036,9 @@
       <c r="E29" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="H29" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1724,6 +2053,9 @@
       <c r="E30" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="H30" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1739,7 +2071,10 @@
         <v>88</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H31" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1756,7 +2091,10 @@
         <v>88</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H32" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1773,10 +2111,13 @@
         <v>88</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H33" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1793,12 +2134,15 @@
         <v>88</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H34" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
         <v>32</v>
@@ -1810,7 +2154,10 @@
         <v>88</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H35" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1827,7 +2174,10 @@
         <v>88</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H36" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1844,7 +2194,10 @@
         <v>88</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1882,7 +2235,7 @@
         <v>33</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1893,10 +2246,13 @@
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1913,7 +2269,7 @@
         <v>87</v>
       </c>
       <c r="H42" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1951,7 +2307,7 @@
         <v>33</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1962,10 +2318,13 @@
         <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1982,7 +2341,7 @@
         <v>87</v>
       </c>
       <c r="H48" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -2020,7 +2379,7 @@
         <v>33</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2031,10 +2390,13 @@
         <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2051,7 +2413,7 @@
         <v>87</v>
       </c>
       <c r="H54" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -2089,7 +2451,7 @@
         <v>33</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2100,10 +2462,13 @@
         <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>87</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2120,7 +2485,7 @@
         <v>87</v>
       </c>
       <c r="H60" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
@@ -2158,21 +2523,24 @@
         <v>33</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C64" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>87</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2180,13 +2548,16 @@
         <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>87</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2227,21 +2598,24 @@
         <v>33</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>87</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2249,13 +2623,16 @@
         <v>44</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>87</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2298,7 +2675,7 @@
         <v>33</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2306,7 +2683,7 @@
         <v>81</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>56</v>
@@ -2315,7 +2692,7 @@
         <v>87</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2323,13 +2700,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C75" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>87</v>
+      </c>
+      <c r="H75" s="20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -2367,7 +2747,7 @@
         <v>33</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2383,6 +2763,9 @@
       <c r="E79" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="H79" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -2397,8 +2780,11 @@
       <c r="E80" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>42</v>
       </c>
@@ -2411,8 +2797,11 @@
       <c r="E81" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
         <v>86</v>
       </c>
@@ -2422,7 +2811,7 @@
       <c r="E84" s="16"/>
       <c r="F84" s="16"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>10</v>
       </c>
@@ -2447,27 +2836,32 @@
     <mergeCell ref="A20:H20"/>
     <mergeCell ref="A77:H77"/>
   </mergeCells>
-  <conditionalFormatting sqref="A20 A39 A45 A51 A57 A77 A62 A3:H19 A79:H87 A21:G21 A40:G40 A46:G46 A52:G52 A58:G58 A78:G78 A67 A72 A74:B74 A22:H38 A76:H76 D74:H74 A41:H44 A47:H50 A53:H56 A59:H61 A64:H66 A69:H71 A75:G75">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+  <conditionalFormatting sqref="A20 A39 A45 A51 A57 A77 A62 A21:G21 A40:G40 A46:G46 A52:G52 A58:G58 A78:G78 A67 A72 A74:B74 A76:H76 A75:G75 A41:H44 A64:H66 A69:H71 A79:H87 A3:H19 A47:H50 A53:H56 A59:H61 D74:H74 A22:H38">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:G63">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:G68">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:G73">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+      <formula>"YES"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H75">
     <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"YES"</formula>
     </cfRule>

</xml_diff>